<commit_message>
Added some requirements to Hardware, will need to review later once design constraints are better known
</commit_message>
<xml_diff>
--- a/Requirements for Rear View Camera.xlsx
+++ b/Requirements for Rear View Camera.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9237dc13137801a8/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9237dc13137801a8/Desktop/Rear_view_Camera/Rear-View-Camera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAB637B1-695F-4410-A1F6-96A575741BE0}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61AC654A-50A8-4119-9010-7EFA26FFFD97}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="12420" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
   <si>
     <t>Hardware</t>
   </si>
@@ -292,6 +292,46 @@
   </si>
   <si>
     <t>F_RVC_28</t>
+  </si>
+  <si>
+    <t>The IR sensor will pass voltage ranges that an IC can read</t>
+  </si>
+  <si>
+    <t>The IR Sensor will be tested using  a power supply and Multimeter.
+The IR sensor will be connected for normal conditions, and move an object closer to the sensor to check the voltage change. Pass if the voltage change as the object moves closer and farther away is verified by the Multimeter</t>
+  </si>
+  <si>
+    <t>The Receiver will be powered by two coin cells</t>
+  </si>
+  <si>
+    <t>Receive will be able to turn on with two coin cells</t>
+  </si>
+  <si>
+    <t>The Transmiter will be powered by two coin cells</t>
+  </si>
+  <si>
+    <t>Transmitter will be able to turn on with two coin cells</t>
+  </si>
+  <si>
+    <t>The speaker will be powered by two coin cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker will be verified by spec sheets and test benching for loading </t>
+  </si>
+  <si>
+    <t>with test bench equipment, passing a voltage less than the rated voltage, the voltage regulator will begin a smooth power down</t>
+  </si>
+  <si>
+    <t>Transmitter will have voltage regulator sensing for smooth power down</t>
+  </si>
+  <si>
+    <t>Receiver will have voltage regulator sensing for smooth power down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR sensor will have over current protection designed to maintain less than 1 A </t>
+  </si>
+  <si>
+    <t>with test bench equipment, passing a 1.1 amp current will see the over current protection to activate</t>
   </si>
 </sst>
 </file>
@@ -384,11 +424,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,173 +724,215 @@
   <dimension ref="C6:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:5" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="7" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="D10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="D11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="D12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="3:5" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -846,150 +940,150 @@
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="3:5" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -997,142 +1091,142 @@
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
+      <c r="C75" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+      <c r="C78" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
+      <c r="C79" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+      <c r="C84" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
+      <c r="C85" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
+      <c r="C86" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
+      <c r="C87" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
+      <c r="C88" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
+      <c r="C89" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
+      <c r="C90" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
+      <c r="C91" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
+      <c r="C92" s="2" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More research on the ESP32, looks like I'll buy the DOIT DEV Kit. added aditional requirement breakdown
</commit_message>
<xml_diff>
--- a/Requirements for Rear View Camera.xlsx
+++ b/Requirements for Rear View Camera.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9237dc13137801a8/Desktop/Rear_view_Camera/Rear-View-Camera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61AC654A-50A8-4119-9010-7EFA26FFFD97}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{104624CB-5927-41FA-8F3E-AE38EFD82004}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="12420" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
   <si>
     <t>Hardware</t>
   </si>
@@ -332,6 +332,21 @@
   </si>
   <si>
     <t>with test bench equipment, passing a 1.1 amp current will see the over current protection to activate</t>
+  </si>
+  <si>
+    <t>Stake holder Requiremenets</t>
+  </si>
+  <si>
+    <t>System Requirements</t>
+  </si>
+  <si>
+    <t>Subsystem Requirements</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>Have the sensor turn on with a touch of my finger?</t>
   </si>
 </sst>
 </file>
@@ -721,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C6:E92"/>
+  <dimension ref="C2:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,9 +748,31 @@
     <col min="3" max="3" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:5" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
@@ -757,7 +794,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
@@ -768,7 +805,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
@@ -779,7 +816,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
@@ -790,7 +827,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
@@ -801,7 +838,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
@@ -812,7 +849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
@@ -823,17 +860,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
added Stake Holder requirements, Will finalize requirements by EOW
</commit_message>
<xml_diff>
--- a/Requirements for Rear View Camera.xlsx
+++ b/Requirements for Rear View Camera.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9237dc13137801a8/Desktop/Rear_view_Camera/Rear-View-Camera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{104624CB-5927-41FA-8F3E-AE38EFD82004}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3C6E71-C308-4A19-AF25-48361A849CA3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="133">
   <si>
     <t>Hardware</t>
   </si>
@@ -340,13 +350,91 @@
     <t>System Requirements</t>
   </si>
   <si>
-    <t>Subsystem Requirements</t>
-  </si>
-  <si>
-    <t>Possible</t>
-  </si>
-  <si>
-    <t>Have the sensor turn on with a touch of my finger?</t>
+    <t>Stakeholder Requirements</t>
+  </si>
+  <si>
+    <t>STKH_RVC_01</t>
+  </si>
+  <si>
+    <t>STKH_RVC_02</t>
+  </si>
+  <si>
+    <t>STKH_RVC_03</t>
+  </si>
+  <si>
+    <t>STKH_RVC_04</t>
+  </si>
+  <si>
+    <t>STKH_RVC_05</t>
+  </si>
+  <si>
+    <t>STKH_RVC_06</t>
+  </si>
+  <si>
+    <t>STKH_RVC_07</t>
+  </si>
+  <si>
+    <t>STKH_RVC_08</t>
+  </si>
+  <si>
+    <t>STKH_RVC_09</t>
+  </si>
+  <si>
+    <t>STKH_RVC_10</t>
+  </si>
+  <si>
+    <t>STKH_RVC_11</t>
+  </si>
+  <si>
+    <t>STKH_RVC_12</t>
+  </si>
+  <si>
+    <t>STKH_RVC_13</t>
+  </si>
+  <si>
+    <t>The System will be small enough to be held in your hands</t>
+  </si>
+  <si>
+    <t>The system will work off of replacable batteries</t>
+  </si>
+  <si>
+    <t>The system will communicate over bluetooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system will notify User of proximity </t>
+  </si>
+  <si>
+    <t>The System will implement adjustable noises to User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The System will have speaker for adjustable noises </t>
+  </si>
+  <si>
+    <t>The System will be portable</t>
+  </si>
+  <si>
+    <t>The System will be water resistant</t>
+  </si>
+  <si>
+    <t>The System will be Magnetic to stick on Vehicle Bumper</t>
+  </si>
+  <si>
+    <t>The System will turn on using human capacitance ( Human Finger Sensing )</t>
+  </si>
+  <si>
+    <t>The System will turn off using human capacitance</t>
+  </si>
+  <si>
+    <t>The System will indicate when it is paired</t>
+  </si>
+  <si>
+    <t>The system will remain paired until turned off</t>
+  </si>
+  <si>
+    <t>Need to trace requirements and add sub system requireements if needed</t>
+  </si>
+  <si>
+    <t>What Stakeholder requirement does this satisfy</t>
   </si>
 </sst>
 </file>
@@ -376,7 +464,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,8 +477,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -435,11 +529,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,6 +584,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,538 +889,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:H92"/>
+  <dimension ref="A2:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="62.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="70.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D2" s="2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E3" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H4" t="s">
+      <c r="B5" s="11"/>
+      <c r="K5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
+      <c r="B6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="B7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="K19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="K20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="K21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="K22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="K23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="K24" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="K25" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="K26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="K27" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="K28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="K29" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="K30" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="K31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="K32" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K33" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K34" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="11:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="K35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="M35" s="5"/>
+      <c r="N35" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="C35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="5" t="s">
+    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K36" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K37" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K38" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K40" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K41" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K42" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K43" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K44" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K45" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K46" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K47" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K48" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K49" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K50" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K51" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K52" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K53" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K54" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K55" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K56" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K57" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K58" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K59" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K60" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K61" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K62" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K63" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="11:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="K64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L64" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="M64" s="5"/>
+      <c r="N64" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C54" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C58" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C62" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C63" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="3:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="C64" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="2" t="s">
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" s="2" t="s">
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" s="2" t="s">
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" s="2" t="s">
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" s="2" t="s">
+    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="2" t="s">
+    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K70" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="2" t="s">
+    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K71" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="2" t="s">
+    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K72" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" s="2" t="s">
+    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C74" s="2" t="s">
+    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K74" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75" s="2" t="s">
+    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K75" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76" s="2" t="s">
+    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K76" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77" s="2" t="s">
+    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K77" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78" s="2" t="s">
+    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K78" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" s="2" t="s">
+    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K79" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" s="2" t="s">
+    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K80" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="2" t="s">
+    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K81" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="2" t="s">
+    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K82" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C83" s="2" t="s">
+    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K83" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" s="2" t="s">
+    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K84" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C85" s="2" t="s">
+    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K85" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="2" t="s">
+    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K86" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C87" s="2" t="s">
+    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K87" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" s="2" t="s">
+    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K88" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" s="2" t="s">
+    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K89" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90" s="2" t="s">
+    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K90" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" s="2" t="s">
+    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K91" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92" s="2" t="s">
+    <row r="92" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K92" s="2" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes for the risk Cube
</commit_message>
<xml_diff>
--- a/Requirements for Rear View Camera.xlsx
+++ b/Requirements for Rear View Camera.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9237dc13137801a8/Desktop/Rear_view_Camera/Rear-View-Camera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F3C6E71-C308-4A19-AF25-48361A849CA3}"/>
+  <xr:revisionPtr revIDLastSave="353" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7A5D311-BF8B-4536-A7C4-4F9DF006BA45}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="143">
   <si>
     <t>Hardware</t>
   </si>
@@ -435,13 +435,43 @@
   </si>
   <si>
     <t>What Stakeholder requirement does this satisfy</t>
+  </si>
+  <si>
+    <t>Risks</t>
+  </si>
+  <si>
+    <t>The system will need to communicate over bluetooth. I have not constructed bluetooth and therefore the consequence of not being able to meet requirment.</t>
+  </si>
+  <si>
+    <t>The team has never used the ESP32 or programmed in a language for embedded systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team has never used capacitance touch buttons. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wireless communication . The team has never done anything over wireless communication </t>
+  </si>
+  <si>
+    <t>Likelihood</t>
+  </si>
+  <si>
+    <t>Consequence</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>Risk Cube</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,8 +493,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,8 +544,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -545,9 +618,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -556,19 +627,36 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -597,17 +685,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,17 +1039,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6" style="7" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="72.140625" style="2" bestFit="1" customWidth="1"/>
@@ -919,29 +1067,35 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="K5" s="13" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="16"/>
+      <c r="K5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="13" t="s">
         <v>118</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1164,69 +1318,213 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
+      <c r="C24" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
       <c r="K24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+    <row r="25" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="20">
+        <v>5</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="36" t="s">
+        <v>141</v>
+      </c>
       <c r="K25" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="25">
+        <v>1</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="20">
+        <v>4</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
       <c r="K26" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="25">
+        <v>2</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="20">
+        <v>3</v>
+      </c>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="31"/>
+      <c r="I27" s="35"/>
       <c r="K27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="25">
+        <v>3</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="20">
+        <v>2</v>
+      </c>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
       <c r="K28" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="25">
+        <v>4</v>
+      </c>
+      <c r="C29" s="27"/>
+      <c r="D29" s="20">
+        <v>1</v>
+      </c>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="32"/>
       <c r="K29" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="6">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6">
+        <v>3</v>
+      </c>
+      <c r="H30" s="6">
+        <v>4</v>
+      </c>
+      <c r="I30" s="17">
+        <v>5</v>
+      </c>
+      <c r="J30" s="24"/>
       <c r="K30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+    <row r="31" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="24"/>
       <c r="K31" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
       <c r="K32" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
       <c r="K33" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
       <c r="K34" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="11:14" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="9"/>
       <c r="K35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1238,67 +1536,68 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E36" s="24"/>
       <c r="K36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K37" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K38" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K39" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K40" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K41" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K42" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K43" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K44" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K45" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K46" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K47" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K48" s="2" t="s">
         <v>45</v>
       </c>
@@ -1531,10 +1830,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="C24:I24"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:C29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
here is my latest work. added some changes to design and current requirement changes
</commit_message>
<xml_diff>
--- a/Requirements for Rear View Camera.xlsx
+++ b/Requirements for Rear View Camera.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9237dc13137801a8/Desktop/Rear_view_Camera/Rear-View-Camera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ABD781C-2E56-40C3-907F-858E38F60F2B}"/>
+  <xr:revisionPtr revIDLastSave="447" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{201CBB20-B6E6-499E-9117-9952E0FF3D9B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="HLD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="189">
   <si>
     <t>Hardware</t>
   </si>
@@ -465,13 +466,151 @@
   </si>
   <si>
     <t>Risk Cube</t>
+  </si>
+  <si>
+    <t>The receiver will accept bluetooth signals within the required frequency</t>
+  </si>
+  <si>
+    <t>The Receiver will translate bluetooth message for ESP .</t>
+  </si>
+  <si>
+    <t>The receiver will convert translation to readable logic for ESP</t>
+  </si>
+  <si>
+    <t>The receiver will compare value of translated value to standard distance measurements</t>
+  </si>
+  <si>
+    <t>the receiver will display an output that signals what stage of distance the value is in</t>
+  </si>
+  <si>
+    <t>The receiver will maintain connection until turned off</t>
+  </si>
+  <si>
+    <t>The receiver will indicate connection is made to tranceiver</t>
+  </si>
+  <si>
+    <t>The receiver will be able to turn off the tranceiver</t>
+  </si>
+  <si>
+    <t>The tranceiver will power distance measuring booster</t>
+  </si>
+  <si>
+    <t>the tranceiver will establish connection to receiver</t>
+  </si>
+  <si>
+    <t>the tranceiver will indicate connection through an LED</t>
+  </si>
+  <si>
+    <t>The tranceiver will accept Bluetooth signals within the required frequency</t>
+  </si>
+  <si>
+    <t>The tranceiver will use ADC to voncert distance booster signal to analog</t>
+  </si>
+  <si>
+    <t>the tranceiver will transmit distance converted value over bluetooth</t>
+  </si>
+  <si>
+    <t>The tranceiver will transmit within milliseconds new values of distance</t>
+  </si>
+  <si>
+    <t>the tranceiver will remain in low power mode until turned on by receiver</t>
+  </si>
+  <si>
+    <t>The receiver will reamin in low power mode until turned on</t>
+  </si>
+  <si>
+    <t>the receiver will be turned off/low power mode by the receiver</t>
+  </si>
+  <si>
+    <t>the tranceiver will have low power modes</t>
+  </si>
+  <si>
+    <t>the receiver will have low power modes</t>
+  </si>
+  <si>
+    <t>tranceiver will have bluetooth modules/libraries</t>
+  </si>
+  <si>
+    <t>receiver will have bluetooth  modules/libraries</t>
+  </si>
+  <si>
+    <t>Magnetic plate for transmitter</t>
+  </si>
+  <si>
+    <t>Capacitive buttons</t>
+  </si>
+  <si>
+    <t>Leds</t>
+  </si>
+  <si>
+    <t>ESP32 pin out ( Transmitter + receiver )</t>
+  </si>
+  <si>
+    <t>Enclosure</t>
+  </si>
+  <si>
+    <t>setup code for initialization</t>
+  </si>
+  <si>
+    <t>loop code for distance values</t>
+  </si>
+  <si>
+    <t>loop code for turning on and off</t>
+  </si>
+  <si>
+    <t>loop code for adc conversion</t>
+  </si>
+  <si>
+    <t>loop code bluetooth connection</t>
+  </si>
+  <si>
+    <t>loop code for decoding bluetooth</t>
+  </si>
+  <si>
+    <t>loop code for transmitting information over bluetooth</t>
+  </si>
+  <si>
+    <t>Transmitter</t>
+  </si>
+  <si>
+    <t>Receiver</t>
+  </si>
+  <si>
+    <t>The ESP32 will take said distance using adc pins</t>
+  </si>
+  <si>
+    <t>The ESP32 will take samples every 5 milliseconds</t>
+  </si>
+  <si>
+    <t>the esp32 will transmit value over bluetooth</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>The distance measure will measure distance</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>how is measuring device setup</t>
+  </si>
+  <si>
+    <t>how do we call adc pins</t>
+  </si>
+  <si>
+    <t>how fast can we send samples/should we store samples</t>
+  </si>
+  <si>
+    <t>how is bluetooth generated and how do we know how fast it'll get there</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +659,13 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -656,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,9 +825,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -691,30 +834,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -727,15 +854,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,14 +884,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,6 +908,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>91769</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93BEB5D8-3280-02D5-F59D-C8BAD10415D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="434340"/>
+          <a:ext cx="9639629" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1039,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,7 +1243,7 @@
     <col min="7" max="7" width="23.88671875" customWidth="1"/>
     <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="72.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="79.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="62.44140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="70.88671875" style="2" customWidth="1"/>
     <col min="17" max="17" width="46.6640625" bestFit="1" customWidth="1"/>
@@ -1067,35 +1258,29 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="5" spans="1:14" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="13"/>
-      <c r="K5" s="34" t="s">
+      <c r="B5" s="29"/>
+      <c r="K5" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>118</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1115,7 +1300,7 @@
       <c r="A7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>119</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -1133,7 +1318,7 @@
       <c r="A8" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>120</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -1150,7 +1335,7 @@
       <c r="A9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>121</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1167,7 +1352,7 @@
       <c r="A10" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>122</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1184,7 +1369,7 @@
       <c r="A11" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>123</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1201,7 +1386,7 @@
       <c r="A12" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>124</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1218,7 +1403,7 @@
       <c r="A13" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>125</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1235,7 +1420,7 @@
       <c r="A14" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>126</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1246,7 +1431,7 @@
       <c r="A15" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>127</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -1257,7 +1442,7 @@
       <c r="A16" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>128</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1268,7 +1453,7 @@
       <c r="A17" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>129</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -1279,7 +1464,7 @@
       <c r="A18" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>130</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1287,66 +1472,60 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
       <c r="K19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
       <c r="K20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
       <c r="K21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
       <c r="K22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
       <c r="K23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
       <c r="K24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37" t="s">
+      <c r="B25" s="22"/>
+      <c r="C25" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="11">
         <v>5</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="26" t="s">
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19" t="s">
         <v>141</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -1354,92 +1533,92 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="13">
         <v>1</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="16">
+      <c r="C26" s="24"/>
+      <c r="D26" s="11">
         <v>4</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
       <c r="K26" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="13">
         <v>2</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="16">
+      <c r="C27" s="24"/>
+      <c r="D27" s="11">
         <v>3</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="27" t="s">
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="25"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="18"/>
       <c r="K27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="13">
         <v>3</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="16">
+      <c r="C28" s="24"/>
+      <c r="D28" s="11">
         <v>2</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
       <c r="K28" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="13">
         <v>4</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="16">
+      <c r="C29" s="24"/>
+      <c r="D29" s="11">
         <v>1</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="22"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="15"/>
       <c r="K29" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="E30" s="6">
         <v>1</v>
       </c>
@@ -1452,79 +1631,53 @@
       <c r="H30" s="6">
         <v>4</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="6">
         <v>5</v>
       </c>
-      <c r="J30" s="18"/>
       <c r="K30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A31" s="6"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="28" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="18"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
       <c r="K31" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
+      <c r="B32" s="8"/>
       <c r="K32" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
+      <c r="B33" s="8"/>
       <c r="K33" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
+      <c r="B34" s="8"/>
       <c r="K34" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
-      <c r="B35" s="9"/>
+      <c r="B35" s="8"/>
       <c r="K35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1537,95 +1690,148 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E36" s="18"/>
       <c r="K36" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K37" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="L37" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K38" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="L38" s="2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K39" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="L39" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K40" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="L40" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K41" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="L41" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K42" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="L42" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K43" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="L43" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K44" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="L44" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K45" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="L45" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K46" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="L46" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K47" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="L47" s="2" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K48" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="L48" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="49" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K49" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="L49" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="50" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K50" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="L50" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="51" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K51" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="L51" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="52" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K52" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="L52" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="53" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K53" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="L53" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="54" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K54" s="2" t="s">
@@ -1689,82 +1895,94 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K65" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="L65" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K66" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="67" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="L66" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K67" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="L67" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K68" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="69" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="L68" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K69" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K70" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K71" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K72" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K73" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K74" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K75" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K76" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K77" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K78" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K79" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K80" s="2" t="s">
         <v>76</v>
       </c>
@@ -1831,6 +2049,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K5:N5"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:C29"/>
@@ -1838,10 +2057,153 @@
     <mergeCell ref="C30:D31"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="K5:N5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2497B31E-59FF-4A09-955A-4801CFBEE1B6}">
+  <dimension ref="B8:S34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="45.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N8" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+    </row>
+    <row r="9" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>165</v>
+      </c>
+      <c r="R9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>166</v>
+      </c>
+      <c r="R10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>167</v>
+      </c>
+      <c r="R11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>168</v>
+      </c>
+      <c r="R12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>169</v>
+      </c>
+      <c r="R13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="R14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="R15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+    </row>
+    <row r="30" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>181</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="H29:J29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
additional research on distance measurer
</commit_message>
<xml_diff>
--- a/Requirements for Rear View Camera.xlsx
+++ b/Requirements for Rear View Camera.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9237dc13137801a8/Desktop/Rear_view_Camera/Rear-View-Camera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="447" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{201CBB20-B6E6-499E-9117-9952E0FF3D9B}"/>
+  <xr:revisionPtr revIDLastSave="456" documentId="11_F25DC773A252ABDACC10487FD91F62F65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{845799AD-97BB-4F46-B661-02B2D42E457F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="191">
   <si>
     <t>Hardware</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>how is bluetooth generated and how do we know how fast it'll get there</t>
+  </si>
+  <si>
+    <t>Part of Git hub repository /under how the measuring device works</t>
+  </si>
+  <si>
+    <t>looking more like 60 ms is going to be our target</t>
   </si>
 </sst>
 </file>
@@ -854,6 +860,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -881,16 +890,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -920,8 +926,8 @@
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>91769</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533729</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
@@ -963,6 +969,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1258,23 +1268,23 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="5" spans="1:14" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="K5" s="30" t="s">
+      <c r="B5" s="30"/>
+      <c r="K5" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
@@ -1497,25 +1507,25 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
       <c r="K24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23" t="s">
+      <c r="B25" s="23"/>
+      <c r="C25" s="24" t="s">
         <v>138</v>
       </c>
       <c r="D25" s="11">
@@ -1539,7 +1549,7 @@
       <c r="B26" s="13">
         <v>1</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="11">
         <v>4</v>
       </c>
@@ -1559,7 +1569,7 @@
       <c r="B27" s="13">
         <v>2</v>
       </c>
-      <c r="C27" s="24"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="11">
         <v>3</v>
       </c>
@@ -1581,7 +1591,7 @@
       <c r="B28" s="13">
         <v>3</v>
       </c>
-      <c r="C28" s="24"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="11">
         <v>2</v>
       </c>
@@ -1601,7 +1611,7 @@
       <c r="B29" s="13">
         <v>4</v>
       </c>
-      <c r="C29" s="24"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="11">
         <v>1</v>
       </c>
@@ -1617,8 +1627,8 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="6">
         <v>1</v>
       </c>
@@ -1641,15 +1651,15 @@
     <row r="31" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A31" s="6"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25" t="s">
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
       <c r="K31" s="2" t="s">
         <v>27</v>
       </c>
@@ -2069,29 +2079,29 @@
   <dimension ref="B8:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="45.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="33" t="s">
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R8" s="33"/>
-      <c r="S8" s="33"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
     </row>
     <row r="9" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O9" t="s">
@@ -2144,34 +2154,40 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="H29" s="31" t="s">
+      <c r="H29" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-    </row>
-    <row r="30" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+    </row>
+    <row r="30" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>183</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="31" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F30" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>179</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>186</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2180,6 +2196,9 @@
       </c>
       <c r="E32" s="7" t="s">
         <v>187</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="3:5" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>